<commit_message>
Enhancement: Added Puducherry Knowledge Base, AI Caching, and UI consistency
</commit_message>
<xml_diff>
--- a/assets/Data Collections/AdventureActivities.xlsx
+++ b/assets/Data Collections/AdventureActivities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vishn\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\TrekBuddy\assets\Data Collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8F9C89-51B1-45A1-A692-8BBB55939CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6126D9-E310-4CBE-912D-5052178547E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cycling" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,23 @@
     <sheet name="Trekking" sheetId="3" r:id="rId3"/>
     <sheet name="Theme Parks" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="159">
   <si>
     <t>Activity Name</t>
   </si>
@@ -100,9 +111,6 @@
     <t>Guide Required</t>
   </si>
   <si>
-    <t>Park Name</t>
-  </si>
-  <si>
     <t>Ticket Price</t>
   </si>
   <si>
@@ -110,16 +118,420 @@
   </si>
   <si>
     <t>Parking Available</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Paradise+Beach+Puducherry</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Nonankuppam</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Chunnambar+Boat+House</t>
+  </si>
+  <si>
+    <t>Pudukuppam</t>
+  </si>
+  <si>
+    <t>Paradise Beach Boat Ride</t>
+  </si>
+  <si>
+    <t>Boating</t>
+  </si>
+  <si>
+    <t>Paradise Beach</t>
+  </si>
+  <si>
+    <t>5:00PM</t>
+  </si>
+  <si>
+    <t>All ages</t>
+  </si>
+  <si>
+    <t>Life Jacket</t>
+  </si>
+  <si>
+    <t>Oct – Mar</t>
+  </si>
+  <si>
+    <t>Boat ride compulsory to reach beach</t>
+  </si>
+  <si>
+    <t>Chunnambar Kayaking</t>
+  </si>
+  <si>
+    <t>Kayaking</t>
+  </si>
+  <si>
+    <t>Chunnambar Backwaters</t>
+  </si>
+  <si>
+    <t>10+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                             0413 260 2444</t>
+  </si>
+  <si>
+    <t>Calm backwater kayaking</t>
+  </si>
+  <si>
+    <t>Serenity Beach Surfing</t>
+  </si>
+  <si>
+    <t>Surfing</t>
+  </si>
+  <si>
+    <t>Serenity Beach</t>
+  </si>
+  <si>
+    <t>Kottakuppam</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Serenity+Beach+Puducherry</t>
+  </si>
+  <si>
+    <t>12+</t>
+  </si>
+  <si>
+    <t>Surfboard, Safety Vest</t>
+  </si>
+  <si>
+    <t>Nov – Feb</t>
+  </si>
+  <si>
+    <t>Ideal for beginners</t>
+  </si>
+  <si>
+    <t>Auroville Beach Swimming</t>
+  </si>
+  <si>
+    <t>Swimming</t>
+  </si>
+  <si>
+    <t>Auroville Beach</t>
+  </si>
+  <si>
+    <t>Auroville</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Auroville+Beach+Puducherry</t>
+  </si>
+  <si>
+    <t>Free</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             -</t>
+  </si>
+  <si>
+    <t>All seasons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                           -</t>
+  </si>
+  <si>
+    <t>Strong waves; caution advised</t>
+  </si>
+  <si>
+    <t>Rock Beach Photography Walk</t>
+  </si>
+  <si>
+    <t>Leisure Activity</t>
+  </si>
+  <si>
+    <t>Rock Beach</t>
+  </si>
+  <si>
+    <t>White Town</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Rock+Beach+Puducherry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                             -</t>
+  </si>
+  <si>
+    <t>Not Required</t>
+  </si>
+  <si>
+    <t>No swimming allowed</t>
+  </si>
+  <si>
+    <t>Promenade Beach Yoga</t>
+  </si>
+  <si>
+    <t>Wellness Activity</t>
+  </si>
+  <si>
+    <t>Promenade Beach</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Promenade+Beach+Puducherry</t>
+  </si>
+  <si>
+    <t>Yoga Mat (Optional)</t>
+  </si>
+  <si>
+    <t>Popular morning wellness activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                           - </t>
+  </si>
+  <si>
+    <t>Mangrove Beach Kayaking</t>
+  </si>
+  <si>
+    <t>Arikamedu</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Mangrove+Kayaking+Puducherry</t>
+  </si>
+  <si>
+    <t>Eco-tourism kayaking experience</t>
+  </si>
+  <si>
+    <t>Promenade Beach Cycling</t>
+  </si>
+  <si>
+    <t>Cycling</t>
+  </si>
+  <si>
+    <t>Rock Beach – Promenade stretch</t>
+  </si>
+  <si>
+    <t>₹100–₹200/hr</t>
+  </si>
+  <si>
+    <t>Early Morning</t>
+  </si>
+  <si>
+    <t>Vehicle-free during mornings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                        -</t>
+  </si>
+  <si>
+    <t>Popular route for tourists</t>
+  </si>
+  <si>
+    <t>Rock Beach Cycling Route</t>
+  </si>
+  <si>
+    <t>Gandhi Statue to War Memorial</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Morning &amp; Evening</t>
+  </si>
+  <si>
+    <t>Avoid peak crowd hours</t>
+  </si>
+  <si>
+    <t>Evening vehicle restriction</t>
+  </si>
+  <si>
+    <t>Auroville Beach Cycling</t>
+  </si>
+  <si>
+    <t>Auroville Main Road to Beach Road</t>
+  </si>
+  <si>
+    <t>₹150–₹300/hr</t>
+  </si>
+  <si>
+    <t>Wear helmet due to uneven roads</t>
+  </si>
+  <si>
+    <t>Scenic coastal ride</t>
+  </si>
+  <si>
+    <t>Serenity Beach Cycling</t>
+  </si>
+  <si>
+    <t>ECR Road to Serenity Beach</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>Watch for sand patches</t>
+  </si>
+  <si>
+    <t>Suitable for experienced cyclists</t>
+  </si>
+  <si>
+    <t>Ousteri Lake Cycling Trail</t>
+  </si>
+  <si>
+    <t>Ousteri</t>
+  </si>
+  <si>
+    <t>Outer Lake Road</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Ousteri+Lake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                             6:00 AM</t>
+  </si>
+  <si>
+    <t>Wildlife crossing possible</t>
+  </si>
+  <si>
+    <t>Calm and nature-friendly route</t>
+  </si>
+  <si>
+    <t>Kadagampattu Nature Trek</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>Kadagampattu Village</t>
+  </si>
+  <si>
+    <t>Forest Trail Loop</t>
+  </si>
+  <si>
+    <t>Thiruvakkarai</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Kadagampattu+Puducherry</t>
+  </si>
+  <si>
+    <t>Uneven terrain; carry water and first-aid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                            -</t>
+  </si>
+  <si>
+    <t>Rural forest trek; suitable for adventure enthusiasts</t>
+  </si>
+  <si>
+    <t>Urban Forest Trail</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Pondicherry Zoos’s Urban Forest</t>
+  </si>
+  <si>
+    <t>Forest Loop</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Pondy+Urban+Forest+Trail</t>
+  </si>
+  <si>
+    <t>Orleanpet</t>
+  </si>
+  <si>
+    <t>1.5 hrs</t>
+  </si>
+  <si>
+    <t>3-4 hrs</t>
+  </si>
+  <si>
+    <t>Yes (recommended)</t>
+  </si>
+  <si>
+    <t>Slippery in monsoon; stay with guide</t>
+  </si>
+  <si>
+    <t>Short forest trail ideal for biodiversity observation</t>
+  </si>
+  <si>
+    <t>91 9442547481</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Park  Name </t>
+  </si>
+  <si>
+    <t>Manjakuppam</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Ocean+Spray+Resort+Puducherry</t>
+  </si>
+  <si>
+    <t>Adventure &amp; Theme Park</t>
+  </si>
+  <si>
+    <t>Ocean Spray Adventure Park</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Rope activities, zipline and outdoor games</t>
+  </si>
+  <si>
+    <t>Chunnambar Boat House</t>
+  </si>
+  <si>
+    <t>Water Adventure Park</t>
+  </si>
+  <si>
+    <t>₹250 onwards</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                        2226744</t>
+  </si>
+  <si>
+    <t>Boating, water sports and kids activities</t>
+  </si>
+  <si>
+    <t>Bharathi Park</t>
+  </si>
+  <si>
+    <t>Recreational Park</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Bharathi+Park+Puducherry</t>
+  </si>
+  <si>
+    <t>Kids</t>
+  </si>
+  <si>
+    <t>Children’s play area and walking paths</t>
+  </si>
+  <si>
+    <t>Botanical Garden Children’s Zone</t>
+  </si>
+  <si>
+    <t>Mini Theme / Eco Park</t>
+  </si>
+  <si>
+    <t>https://maps.google.com/?q=Botanical+Garden+Puducherry</t>
+  </si>
+  <si>
+    <t>Toy train and children-friendly rides</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;₹&quot;\ #,##0;[Red]&quot;₹&quot;\ \-#,##0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,13 +554,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,18 +879,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M1048576"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="13" width="25.7109375" customWidth="1"/>
+    <col min="1" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.21875" customWidth="1"/>
+    <col min="5" max="5" width="51.77734375" customWidth="1"/>
+    <col min="6" max="6" width="27.5546875" customWidth="1"/>
+    <col min="7" max="12" width="25.6640625" customWidth="1"/>
+    <col min="13" max="13" width="28.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,25 +936,244 @@
         <v>12</v>
       </c>
     </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="H3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4" t="s">
+        <v>91</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" t="s">
+        <v>107</v>
+      </c>
+      <c r="L5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="H6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K6" t="s">
+        <v>114</v>
+      </c>
+      <c r="L6" t="s">
+        <v>91</v>
+      </c>
+      <c r="M6" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{7ED8A252-9D90-4DD7-94F5-A84525DD1A5D}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{095784B9-338B-4B58-A144-53A0E884F0E1}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{B6695310-CD8C-42E1-B1FE-880073523441}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{8F165E64-D155-42E0-977A-1A2884445DBA}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{0B355A88-85D9-4401-B7A7-BD7A73D79697}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="13" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.77734375" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="52.44140625" customWidth="1"/>
+    <col min="6" max="12" width="25.6640625" customWidth="1"/>
+    <col min="13" max="13" width="34.88671875" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,25 +1214,339 @@
         <v>12</v>
       </c>
     </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="6">
+        <v>300</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="5">
+        <v>6384481000</v>
+      </c>
+      <c r="M2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="H3" s="6">
+        <v>800</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1500</v>
+      </c>
+      <c r="I4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="5">
+        <v>8460394496</v>
+      </c>
+      <c r="M4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="H5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" t="s">
+        <v>63</v>
+      </c>
+      <c r="L5" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" t="s">
+        <v>78</v>
+      </c>
+      <c r="K7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1200</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="5">
+        <v>9843555900</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E26" s="5"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{F8C36BC2-A4D2-4305-929E-073CDAB25B10}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{5983A49F-EBDA-4E7B-A97A-1037B49BC723}"/>
+    <hyperlink ref="L2" r:id="rId3" display="AdventureActivities.xlsx" xr:uid="{AFA095BC-A2CC-470D-8511-9CD1B8000992}"/>
+    <hyperlink ref="L3" r:id="rId4" xr:uid="{ECE38B4E-4C37-4434-B2B1-A6D87865D711}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{B087ADCA-D951-4FDF-952F-FE012F78B7FC}"/>
+    <hyperlink ref="L4" r:id="rId6" display="AdventureActivities.xlsx" xr:uid="{00F3E952-D5FF-4047-906D-8D649DE0E9F7}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{D93C9E9C-3489-42D9-9934-586D4BFE7888}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{7DB058CC-D83A-4299-9DB4-F9B23212278C}"/>
+    <hyperlink ref="E7" r:id="rId9" xr:uid="{1F8B383C-8E8D-4F05-9480-7182FD2B226F}"/>
+    <hyperlink ref="E8" r:id="rId10" xr:uid="{F53093F5-5CE0-45CA-AD1F-26EBBF5B54D8}"/>
+    <hyperlink ref="L8" r:id="rId11" display="AdventureActivities.xlsx" xr:uid="{F64A1579-C983-4242-AE69-A4A2070289D5}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L1048576"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="12" width="25.7109375" customWidth="1"/>
+    <col min="1" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
+    <col min="4" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="49.109375" customWidth="1"/>
+    <col min="7" max="9" width="25.6640625" customWidth="1"/>
+    <col min="10" max="10" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" customWidth="1"/>
+    <col min="12" max="12" width="43.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -616,27 +1584,113 @@
         <v>12</v>
       </c>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" t="s">
+        <v>123</v>
+      </c>
+      <c r="L2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="J3" t="s">
+        <v>134</v>
+      </c>
+      <c r="K3" t="s">
+        <v>136</v>
+      </c>
+      <c r="L3" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{57D3BD65-08DD-4779-B413-0158477186F6}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{17CE7C0F-5B07-4708-A7E2-3AB4ABC78492}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="11" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.77734375" customWidth="1"/>
+    <col min="2" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="8" max="10" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -654,13 +1708,13 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
-      </c>
-      <c r="I1" t="s">
-        <v>28</v>
       </c>
       <c r="J1" t="s">
         <v>11</v>
@@ -669,7 +1723,156 @@
         <v>12</v>
       </c>
     </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="G2" s="2">
+        <v>500</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="4">
+        <v>9003945678</v>
+      </c>
+      <c r="K2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" t="s">
+        <v>153</v>
+      </c>
+      <c r="I4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G5" s="2">
+        <v>20</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{5DFF95C6-C108-46F5-B8F6-B68CAD35D66D}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{76F7D8CB-C20E-42EA-87F2-9A39B882AAFA}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>